<commit_message>
Se agrega la seleccion de variables y la calibracion de modelos de clustering
</commit_message>
<xml_diff>
--- a/Data/DIVIPOLA_Municipios.xlsx
+++ b/Data/DIVIPOLA_Municipios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/jd_garciac123_uniandes_edu_co/Documents/4. CUARTO SEMESTRE/Proyecto Analytics 2/ProyectoGerenciaProyectosAnaliticos/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_6837570E0CF0993A848EE59A1DC56F72F5254862" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F3F955-178B-449D-83C9-67CD2C09441A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_6837570E0CF0993A848EE59A1DC56F72F5254862" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74CD5BBA-7090-465E-919D-6692BC15C595}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7227,7 +7227,7 @@
   <dimension ref="A1:XFB1132"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26344,6 +26344,7 @@
     <row r="1131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <autoFilter ref="A1:E1123" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>